<commit_message>
Update prescricoes.xlsx with new data
</commit_message>
<xml_diff>
--- a/Prescrição_python/prescricoes.xlsx
+++ b/Prescrição_python/prescricoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ac289667d0e8ccd/Documentos/Saúde/Prescrições/Prescrição_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="629" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA7B2315-9FA6-432C-AC65-9AD3FBB06B41}"/>
+  <xr:revisionPtr revIDLastSave="728" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1814007-E0DE-4F7A-99C4-91AC35F2CE14}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="4" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
   </bookViews>
   <sheets>
     <sheet name="Medicamentos" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="394">
   <si>
     <t>NomeBusca</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Paracetamol</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Paracetamol 500 mg ___________________ 1 caixa
-Tomar 1 comprimido de 6 em 6 horas se dor ou febre
-Obs. 1: Se não melhora somente com o paracetamol, continue tomando-o junto com o 
-anti-inflamatório abaixo </t>
-  </si>
-  <si>
     <t>Diclofenaco</t>
   </si>
   <si>
@@ -105,14 +99,6 @@
     <t>Analgésico opioide</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Codeina 30 mg _______________ 1 caixa
-Tomar 1 comprimido de 6 em 6 horas se dor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Naproxeno 500 mg ________________________ 1 caixa
-Tomar 1 comprimido de 12 em 12 horas por até 5 dias </t>
-  </si>
-  <si>
     <t>1 – Naproxeno 250 mg ______________________1 caixa
 Tomar 1 comprimido de 12 em 12 horas por até 5 dias</t>
   </si>
@@ -120,10 +106,6 @@
     <t>Escopolamina</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Escopolamina 10 mg _______________ 1 caixa
-Tomar 1 comprimido de 6 em 6 horas se dor </t>
-  </si>
-  <si>
     <t>Antiespasmódico</t>
   </si>
   <si>
@@ -133,14 +115,7 @@
     <t>Domperidona</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Domperidona 10 mg ___________________ 1 caixa
-Tomar 1 comprimido de 8 em 8 horas. Tomar 15-30 minutos antes das refeições </t>
-  </si>
-  <si>
     <t>Doenca</t>
-  </si>
-  <si>
-    <t>Gastrite</t>
   </si>
   <si>
     <t>dor</t>
@@ -162,10 +137,6 @@
     <t>Soro fisiológico</t>
   </si>
   <si>
-    <t>1 - Soro fisiológico 
-Realizar lavagem nasal com soro. Usar seringa</t>
-  </si>
-  <si>
     <t>Budesonida</t>
   </si>
   <si>
@@ -173,23 +144,6 @@
 Aplicar 1 jato em cada narina de 12 em 12 horas por no máximo 7 dias</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Dipirona 500 mg _______________________ 1 caixa
-Tomar 1 comprimido de 6 em 6 horas se dor ou febre
-Obs.: Pode tomar até 2 comprimidos de 6 em 6 horas
-Obs. 2: Se não melhora somente com a dipirona, continue tomando-a junto com o anti-inflamatório abaixo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Paracetamol 750 mg ___________________ 1 caixa
-Tomar 1 comprimido de 6 em 6 horas se dor ou febre
-Obs. 1: Se não melhora somente com o paracetamol, continue tomando-o junto com o anti-inflamatório abaixo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Dipirona 500 mg/ml _____________________ 1 caixa
-Tomar 20 gotas de 6 em 6 horas se dor ou febre
-Obs.: Pode tomar até 40 gotas de 6 em 6 horas
-Obs. 2: Se não melhora somente com a dipirona, continue tomando-a junto com o anti-inflamatório abaixo </t>
-  </si>
-  <si>
     <t>1 - Budesonida spray nasal 50 mcg _______________ 1 frasco
 Aplicar 1 jato em cada narina de 12 em 12 horas por no máximo 7 dias</t>
   </si>
@@ -197,11 +151,6 @@
     <t>Nafazolina</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Nafazolina 0,5mg/ml solução nasal _____________ 1 frasco
-Aplicar 4 gotas “dentro de cada nariz” de 6 em 6 horas por até 5 dias 
-Obs.: Não fazer uso prolongado desta medicação. </t>
-  </si>
-  <si>
     <t>Salbutamol</t>
   </si>
   <si>
@@ -235,10 +184,6 @@
 Infundir 1 colher de sopa (3 g) para cada 150ml de água. Tomar 3 vezes ao dia</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Guaco tintura ______________________ 1 frasco
-Aplicar 40 gotas em um pouco de água e tomar de 8 em 8 horas </t>
-  </si>
-  <si>
     <t>1 – Guaco xarope ______________________ 1 frasco
 Tomar 10 ml de 8 em 8 horas por 5 dias</t>
   </si>
@@ -276,12 +221,6 @@
     <t>Anti-histamínico</t>
   </si>
   <si>
-    <t>gripe</t>
-  </si>
-  <si>
-    <t>resfriado, dor</t>
-  </si>
-  <si>
     <t>infecção</t>
   </si>
   <si>
@@ -388,15 +327,7 @@
 Tomar 1 comprimido de 12 em 12 horas por ___ dias</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Ciprofloxacino 500 mg _____________________ ___ comprimidos
-Tomar 1 comprimido de 12 em 12 horas por ___ dias  </t>
-  </si>
-  <si>
     <t>Ceftriaxona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Ceftriaxona 1 g, 2 g (2 amp) em 100 ml de S.F. 0,9%, EV, correr em 30 minutos, 24/24h, por ___ dias
-Indicação: </t>
   </si>
   <si>
     <t>Fosfomicina</t>
@@ -410,10 +341,6 @@
   </si>
   <si>
     <t>Nitrofurantoína</t>
-  </si>
-  <si>
-    <t>1 – Nitrofurantoina 100 mg __________ __ comprimidos 
-Tomar 1 comprimido de 6 em 6 horas por __ dias</t>
   </si>
   <si>
     <t>Sacarato de hidróxido férrico</t>
@@ -734,10 +661,6 @@
 Tomar 1 comprimido. Dose única</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Metronidazol 10% _________ 1 tubo
-Usar 1 aplicar a noite por 5 dias </t>
-  </si>
-  <si>
     <t>Carmelose</t>
   </si>
   <si>
@@ -761,13 +684,6 @@
     <t>Antisséptico</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Prednisolona 3 mg/ml _____________ 1 caixa
-Tomar 14 ml por dia por 5 dias </t>
-  </si>
-  <si>
-    <t>asma, bronquite</t>
-  </si>
-  <si>
     <t>Nimesulida</t>
   </si>
   <si>
@@ -812,9 +728,6 @@
 Diluir 1 envelope em 1 litro de água fervida ou filtrada. Tomar 1 copo para cada evacuação ou vômitos</t>
   </si>
   <si>
-    <t xml:space="preserve">Eletrólitos </t>
-  </si>
-  <si>
     <t>diarreia</t>
   </si>
   <si>
@@ -842,10 +755,6 @@
   </si>
   <si>
     <t>Ondansetrona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Ondansetrona 4 mg _______________ 20 cp
-Tomar 1 comprimido de 8 em 8 horas se náuseas ou vômitos </t>
   </si>
   <si>
     <t>Dexametasona</t>
@@ -884,10 +793,6 @@
     <t>Exame na dengue</t>
   </si>
   <si>
-    <t>1 - Sais de reidratação oral ________________ _ envelopes
-Para preparar o soro de reidratação oral: diluir 1 envelope em 1 litro de água fervida ou filtrada. Tomar ___ L por dia de soro de reidratação oral. Tomar também líquido caseiros (água, suco, soro caseiro, chá e outros):  ___ L. Total de litros por dia ___ L.) Tomar essa quantidade depois de dois dias de estar sem febre.</t>
-  </si>
-  <si>
     <t>dengue</t>
   </si>
   <si>
@@ -911,10 +816,6 @@
 Inalar 1 puffs por dia</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Beclometasona 50 mcg aerossol _____________ 1 frasco
-Inalar 4 jatos de 12 em 12 horas por dia </t>
-  </si>
-  <si>
     <t>Beclometasona</t>
   </si>
   <si>
@@ -922,10 +823,6 @@
 Inalar 1 jato de 12 em 12 horas por dia</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Beclometasona 250 mcg aerossol ___________ 1 frasco
-Inalar 1 jato de 12 em 12 horas por dia </t>
-  </si>
-  <si>
     <t>Formoterol</t>
   </si>
   <si>
@@ -959,10 +856,6 @@
   </si>
   <si>
     <t>Hidroxiquinolina, trolamina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – Hidroxiquinolina + trolamina otológico (0,4 + 140 mg) __________ 1 frasco
-Aplicar 3 gotas no ouvido afetado de 8 em 8 horas por 5 dias </t>
   </si>
   <si>
     <t>rolha de cerumem</t>
@@ -1041,10 +934,6 @@
     <t>Permanganato de potássio</t>
   </si>
   <si>
-    <t>Diluir 1 envelope em 3 litros de água morna. Realizar banho ou compressa, 3x ao dia. Evitar 
-contato com região de mucosa (olhos e boca por exemplo)</t>
-  </si>
-  <si>
     <t>Mupirocina</t>
   </si>
   <si>
@@ -1133,9 +1022,6 @@
 Tomar 1 comprimido de 8 em 8 horas por 7 dias</t>
   </si>
   <si>
-    <t xml:space="preserve">Flunarizina </t>
-  </si>
-  <si>
     <t>1 – Flunarizina 10 mg ____________ 1 caixa
 Tomar 1 comprimido por dia por 7 dias</t>
   </si>
@@ -1161,12 +1047,6 @@
     <t>Cetoconazol</t>
   </si>
   <si>
-    <t>1 – Cetoconazol 2% xampu __________________________ 1 frasco
-Lavar o couro cabeludo e demais lesões 3 a 4 vezes por semana na crise
-Lavar o couro cabeludo e demais lesões 1 a 2 vezes por semana fora da crise 
-Deixar agir por 3 a 5 minutos antes de enxaguar</t>
-  </si>
-  <si>
     <t>tinea</t>
   </si>
   <si>
@@ -1197,10 +1077,6 @@
     <t>Clortalidona</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Clortalidona 25 mg _________________ 30 cp/mês
-Tomar 1 comprimido por dia pela manhã </t>
-  </si>
-  <si>
     <t>Espironolactona</t>
   </si>
   <si>
@@ -1224,10 +1100,6 @@
     <t>has, ic</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Losartana 50 mg __________________ 60 cp/mês
-Tomar 1 comprimido de 12 em 12 horas </t>
-  </si>
-  <si>
     <t>Anti-hipertensivo, IECA</t>
   </si>
   <si>
@@ -1238,10 +1110,6 @@
 Tomar 1 comprimido por dia</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Enalapril 10 mg ___________________ 60 cp/mês
-Tomar 1 comprimido de 12 em 12 horas </t>
-  </si>
-  <si>
     <t>Metoprolol</t>
   </si>
   <si>
@@ -1296,19 +1164,10 @@
 Tomar 1 comprimido de 12 em 12 horas</t>
   </si>
   <si>
-    <t xml:space="preserve">Albendazol </t>
-  </si>
-  <si>
     <t>1 – Albendazol 400 mg ______ 3 cp
 Tomar 1 comprimido por dia por 3 dias</t>
   </si>
   <si>
-    <t>Helmintoses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitazoxanida </t>
-  </si>
-  <si>
     <t>1 – Nitazoxanida 500 mg _____ 1 cp
 Tomar 1 comprimido de 12 em 12 horas por 3 dias</t>
   </si>
@@ -1320,10 +1179,6 @@
   </si>
   <si>
     <t>Clindamicina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Clindamicina 300 mg ______ ___ comprimidos
-Tomar 1 comprimido de 8 em 8 horas por ___ dias </t>
   </si>
   <si>
     <t>Antibiótico, lincosamida</t>
@@ -1412,24 +1267,7 @@
 Aplicar ___ antes da janta</t>
   </si>
   <si>
-    <t xml:space="preserve">Metformina </t>
-  </si>
-  <si>
-    <t>1 – Metformina 850 mg  ____________________ 30 cp/mês
-Tomar 1 comprimido após o almoço</t>
-  </si>
-  <si>
     <t>Biguanida</t>
-  </si>
-  <si>
-    <t>1 – Metformina 850 mg  ____________________ 60 cp/mês
-Tomar 1 comprimido no café da manhã e 1 comprimido no jantar</t>
-  </si>
-  <si>
-    <t>1 – Metformina 850 mg  ____________________ 90 cp/mês
-Tomar 1 comprimido no café da manhã
-Tomar 1 comprimido no almoço
-Tomar 1 comprimido no jantar</t>
   </si>
   <si>
     <t>Gliclazida</t>
@@ -1534,12 +1372,197 @@
   <si>
     <t>Paciente em leito de sala amarela, tranquilo, contactuante e acompanhado de. Está estável hemodinamicamente e eupneico em a.a. Há boa dieta via oral. Eliminações de fezes adequadas. Diurese em de bom aspecto e adequada. Apresenta bons sinais vitais e sem disglicemias. Nega dor.</t>
   </si>
+  <si>
+    <t>Albendazol</t>
+  </si>
+  <si>
+    <t>Nitazoxanida</t>
+  </si>
+  <si>
+    <t>Flunarizina</t>
+  </si>
+  <si>
+    <t>Metformina</t>
+  </si>
+  <si>
+    <t>1 – Naproxeno 500 mg ________________________ 1 caixa
+Tomar 1 comprimido de 12 em 12 horas por até 5 dias</t>
+  </si>
+  <si>
+    <t>1 – Dipirona 500 mg _______________________ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor ou febre
+Obs.: Pode tomar até 2 comprimidos de 6 em 6 horas
+Obs. 2: Se não melhora somente com a dipirona, continue tomando-a junto com o anti-inflamatório abaixo</t>
+  </si>
+  <si>
+    <t>1 – Dipirona 500 mg/ml _____________________ 1 caixa
+Tomar 20 gotas de 6 em 6 horas se dor ou febre
+Obs.: Pode tomar até 40 gotas de 6 em 6 horas
+Obs. 2: Se não melhora somente com a dipirona, continue tomando-a junto com o anti-inflamatório abaixo</t>
+  </si>
+  <si>
+    <t>1 – Paracetamol 500 mg ___________________ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor ou febre
+Obs. 1: Se não melhora somente com o paracetamol, continue tomando-o junto com o
+anti-inflamatório abaixo</t>
+  </si>
+  <si>
+    <t>1 – Paracetamol 750 mg ___________________ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor ou febre
+Obs. 1: Se não melhora somente com o paracetamol, continue tomando-o junto com o anti-inflamatório abaixo</t>
+  </si>
+  <si>
+    <t>1 – Codeina 30 mg _______________ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor</t>
+  </si>
+  <si>
+    <t>1 – Nitrofurantoina 100 mg __________ __ comprimidos
+Tomar 1 comprimido de 6 em 6 horas por __ dias</t>
+  </si>
+  <si>
+    <t>1 – Ceftriaxona 1 g, 2 g (2 amp) em 100 ml de S.F. 0,9%, EV, correr em 30 minutos, 24/24h, por ___ dias
+Indicação:</t>
+  </si>
+  <si>
+    <t>1 - Clindamicina 300 mg ______ ___ comprimidos
+Tomar 1 comprimido de 8 em 8 horas por ___ dias</t>
+  </si>
+  <si>
+    <t>1 – Ciprofloxacino 500 mg _____________________ ___ comprimidos
+Tomar 1 comprimido de 12 em 12 horas por ___ dias</t>
+  </si>
+  <si>
+    <t>1 – Ondansetrona 4 mg _______________ 20 cp
+Tomar 1 comprimido de 8 em 8 horas se náuseas ou vômitos</t>
+  </si>
+  <si>
+    <t>1 – Escopolamina 10 mg _______________ 1 caixa
+Tomar 1 comprimido de 6 em 6 horas se dor</t>
+  </si>
+  <si>
+    <t>1 – Cetoconazol 2% xampu __________________________ 1 frasco
+Lavar o couro cabeludo e demais lesões 3 a 4 vezes por semana na crise
+Lavar o couro cabeludo e demais lesões 1 a 2 vezes por semana fora da crise
+Deixar agir por 3 a 5 minutos antes de enxaguar</t>
+  </si>
+  <si>
+    <t>1 – Clortalidona 25 mg _________________ 30 cp/mês
+Tomar 1 comprimido por dia pela manhã</t>
+  </si>
+  <si>
+    <t>1 – Losartana 50 mg __________________ 60 cp/mês
+Tomar 1 comprimido de 12 em 12 horas</t>
+  </si>
+  <si>
+    <t>1 – Enalapril 10 mg ___________________ 60 cp/mês
+Tomar 1 comprimido de 12 em 12 horas</t>
+  </si>
+  <si>
+    <t>1 – Metronidazol 10% _________ 1 tubo
+Usar 1 aplicar a noite por 5 dias</t>
+  </si>
+  <si>
+    <t>Diluir 1 envelope em 3 litros de água morna. Realizar banho ou compressa, 3x ao dia. Evitar
+contato com região de mucosa (olhos e boca por exemplo)</t>
+  </si>
+  <si>
+    <t>1 – Beclometasona 50 mcg aerossol _____________ 1 frasco
+Inalar 4 jatos de 12 em 12 horas por dia</t>
+  </si>
+  <si>
+    <t>1 – Prednisolona 3 mg/ml _____________ 1 caixa
+Tomar 14 ml por dia por 5 dias</t>
+  </si>
+  <si>
+    <t>1 - Nafazolina 0,5mg/ml solução nasal _____________ 1 frasco
+Aplicar 4 gotas “dentro de cada nariz” de 6 em 6 horas por até 5 dias
+Obs.: Não fazer uso prolongado desta medicação.</t>
+  </si>
+  <si>
+    <t>1 - Sais de reidratação oral ________________ _ envelopes
+Para preparar o soro de reidratação oral: diluir 1 envelope em 1 litro de água fervida ou filtrada. Tomar ___ L por dia de soro de reidratação oral. Tomar também líquido caseiros (água, suco, soro caseiro, chá e outros): ___ L. Total de litros por dia ___ L.) Tomar essa quantidade depois de dois dias de estar sem febre.</t>
+  </si>
+  <si>
+    <t>1 – Hidroxiquinolina + trolamina otológico (0,4 + 140 mg) __________ 1 frasco
+Aplicar 3 gotas no ouvido afetado de 8 em 8 horas por 5 dias</t>
+  </si>
+  <si>
+    <t>1 – Guaco tintura ______________________ 1 frasco
+Aplicar 40 gotas em um pouco de água e tomar de 8 em 8 horas</t>
+  </si>
+  <si>
+    <t>1 – Domperidona 10 mg ___________________ 1 caixa
+Tomar 1 comprimido de 8 em 8 horas. Tomar 15-30 minutos antes das refeições</t>
+  </si>
+  <si>
+    <t>1 - Soro fisiológico
+Realizar lavagem nasal com soro. Usar seringa</t>
+  </si>
+  <si>
+    <t>1 – Metformina 850 mg ____________________ 30 cp/mês
+Tomar 1 comprimido após o almoço</t>
+  </si>
+  <si>
+    <t>1 – Metformina 850 mg ____________________ 60 cp/mês
+Tomar 1 comprimido no café da manhã e 1 comprimido no jantar</t>
+  </si>
+  <si>
+    <t>1 – Metformina 850 mg ____________________ 90 cp/mês
+Tomar 1 comprimido no café da manhã
+Tomar 1 comprimido no almoço
+Tomar 1 comprimido no jantar</t>
+  </si>
+  <si>
+    <t>Eletrólitos</t>
+  </si>
+  <si>
+    <t>Realizo antissepsia de ferida. Realizo sutura de forma asséptica. Oriento sobre complicações de ferida. Oriento sobre cuidados de ferida. Prescrevo analgesia; Forneço ___ dias de atestado; Retirada de ponto com ___ dias; Oriento sobre checagem de cartão vacinal para verificar nova dose de vacina de tétano</t>
+  </si>
+  <si>
+    <t>Ambroxol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Ambroxol 6 mg/ml ____________ 1 frasco
+Tomar 5 ml de 8 em 8 horas </t>
+  </si>
+  <si>
+    <t>Acetilcisteína</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Acetilcisteína 20 mg/ml _________ 1 frasco
+Tomar 10 ml de 8 em 8 horas </t>
+  </si>
+  <si>
+    <t>Mucolítico</t>
+  </si>
+  <si>
+    <t>Ácido tranexâmico</t>
+  </si>
+  <si>
+    <t>1 - Ácido tranexâmico 500 mg _________ 1 caixa
+Tomar 1 comprimido de 8 em 8 horas por 3 dias</t>
+  </si>
+  <si>
+    <t>Antifibrinolítico</t>
+  </si>
+  <si>
+    <t>menorreia</t>
+  </si>
+  <si>
+    <t>OrdemPrioridade</t>
+  </si>
+  <si>
+    <t>crise asma</t>
+  </si>
+  <si>
+    <t>crise asma, bronquite</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1555,6 +1578,20 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFD8DEE9"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1582,7 +1619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1614,16 +1651,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1707,17 +1748,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}" name="Tabela1" displayName="Tabela1" ref="A1:D131" totalsRowShown="0">
-  <autoFilter ref="A1:D131" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D117">
-    <sortCondition ref="C1:C117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}" name="Tabela1" displayName="Tabela1" ref="A1:E134" totalsRowShown="0">
+  <autoFilter ref="A1:E134" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E134">
+    <sortCondition ref="D1:D134"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FF9AC4B3-0AB1-43C0-813C-9F0FBFCD27C3}" name="NomeBusca" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{A4280A1D-29DF-4DF8-BAEB-74D735392255}" name="PrescricaoCompleta" dataDxfId="22"/>
     <tableColumn id="3" xr3:uid="{1C09888C-F0B3-445C-96A7-59EF6CBB8977}" name="Categoria" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{E1DAEFD1-96A5-4769-95CA-789E157CF235}" name="Doenca" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00D107C9-5770-4523-8A77-BC2E8CCDFA3F}" name="OrdemPrioridade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1760,12 +1806,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C12" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C13" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2E3E19EF-E8C4-4174-A6DD-FE62A883B65B}" name="NomeBusca" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2089,10 +2135,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE9DEBA-C453-4102-816C-FDB2AD0D57A3}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2149,7 @@
     <col min="4" max="4" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2114,1833 +2160,2035 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C72" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B73" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="D75" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="C76" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C77" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="D77" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="D79" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="1" t="s">
+    </row>
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B69" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>252</v>
-      </c>
       <c r="C80" s="4" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>330</v>
+        <v>271</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>330</v>
+        <v>271</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>224</v>
+        <v>293</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>49</v>
+        <v>292</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>50</v>
+        <v>272</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>49</v>
+        <v>279</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>50</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>227</v>
+        <v>288</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>51</v>
+        <v>283</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>41</v>
+        <v>301</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>51</v>
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>222</v>
+        <v>302</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>36</v>
+        <v>290</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>223</v>
+        <v>291</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>49</v>
+        <v>292</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>211</v>
+        <v>281</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>49</v>
+        <v>282</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>212</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>213</v>
+        <v>280</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>214</v>
+        <v>365</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>49</v>
+        <v>282</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>212</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>47</v>
+        <v>285</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>48</v>
+        <v>286</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>49</v>
+        <v>284</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>47</v>
+        <v>285</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>184</v>
+        <v>366</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>49</v>
+        <v>284</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>280</v>
+        <v>347</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>281</v>
+        <v>303</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>49</v>
+        <v>305</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>212</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>47</v>
+        <v>348</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>49</v>
+        <v>305</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>294</v>
+        <v>222</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>259</v>
+        <v>152</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>257</v>
+        <v>313</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>258</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>255</v>
+        <v>77</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>256</v>
+        <v>78</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>257</v>
+        <v>309</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>164</v>
+        <v>309</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>197</v>
+        <v>79</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>198</v>
+        <v>80</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>199</v>
+        <v>311</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>218</v>
+        <v>358</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>199</v>
+        <v>310</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>237</v>
+        <v>307</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>238</v>
+        <v>359</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>269</v>
+        <v>83</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>269</v>
+        <v>83</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>291</v>
+        <v>360</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>328</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>56</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>201</v>
+        <v>89</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>202</v>
+        <v>357</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>203</v>
+        <v>6</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
-        <v>245</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>241</v>
+        <v>154</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>242</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>387</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>243</v>
+        <v>388</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>203</v>
+        <v>389</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>204</v>
+        <v>390</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>179</v>
+        <v>66</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C116" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>34</v>
+        <v>185</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>35</v>
+        <v>186</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>351</v>
+        <v>187</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>353</v>
+        <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>364</v>
+        <v>49</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>354</v>
+        <v>50</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>355</v>
+        <v>46</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>356</v>
+        <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>364</v>
+        <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>357</v>
+        <v>45</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>355</v>
+        <v>46</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>364</v>
+        <v>29</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>358</v>
+        <v>30</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>355</v>
+        <v>38</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>356</v>
+        <v>40</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>364</v>
+        <v>29</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>359</v>
+        <v>31</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>355</v>
+        <v>38</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>364</v>
+        <v>32</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>355</v>
+        <v>147</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>364</v>
+        <v>28</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>355</v>
+        <v>28</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>363</v>
+        <v>212</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>355</v>
+        <v>294</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>356</v>
+        <v>213</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="B126" s="3" t="s">
-        <v>366</v>
-      </c>
       <c r="C126" s="4" t="s">
-        <v>355</v>
+        <v>155</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>360</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>368</v>
+        <v>42</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>369</v>
+        <v>148</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>356</v>
+        <v>44</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>369</v>
+        <v>148</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>371</v>
+        <v>43</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>369</v>
+        <v>148</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>374</v>
+        <v>148</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>356</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3965,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
@@ -3973,57 +4221,57 @@
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4054,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
@@ -4062,35 +4310,35 @@
     </row>
     <row r="2" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="265.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="405" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4121,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
@@ -4129,79 +4377,79 @@
     </row>
     <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="405" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4214,10 +4462,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39D3372-8E60-46D2-8A5A-AF4F9411474D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4232,131 +4480,142 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="405" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="405" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>382</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>